<commit_message>
Dropdowns for global objects
</commit_message>
<xml_diff>
--- a/DesktopClient/Dropdowns.xlsx
+++ b/DesktopClient/Dropdowns.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>Call center</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Organization administration</t>
+  </si>
+  <si>
+    <t>DAX.OpenModule.module</t>
   </si>
   <si>
     <t>Accounts receivable</t>
@@ -448,165 +451,257 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="$A$2" sqref="$A$2:$A$30"/>
+      <selection activeCell="$A$2" sqref="$A$2:$A$2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625"/>
+    <col min="1" max="1" width="41.50390625" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625"/>
+    <col min="3" max="3" width="31.36328125" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>13</v>
       </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>10</v>
       </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>18</v>
       </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>20</v>
       </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>24</v>
       </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
         <v>19</v>
       </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
         <v>12</v>
       </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
         <v>5</v>
       </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
         <v>1</v>
       </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
         <v>17</v>
       </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
         <v>22</v>
       </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
         <v>0</v>
       </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
         <v>16</v>
       </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
         <v>6</v>
       </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
         <v>14</v>
       </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
         <v>25</v>
       </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
         <v>4</v>
       </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>